<commit_message>
save results from reconftest
</commit_message>
<xml_diff>
--- a/PV_HC_feeders_with_start.xlsx
+++ b/PV_HC_feeders_with_start.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KERCKHOS\Code\HCobjective\HostingCapacityLVDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0D5833-266D-4F4A-90A0-1F6D0F662702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D708B9DD-1C7B-45A9-9A34-F5869D556B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{408A2332-391D-4F6F-9098-FC4D3D874A52}"/>
+    <workbookView xWindow="2240" yWindow="2240" windowWidth="14400" windowHeight="7360" xr2:uid="{408A2332-391D-4F6F-9098-FC4D3D874A52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="277">
   <si>
     <t>conf</t>
   </si>
@@ -862,6 +862,9 @@
   </si>
   <si>
     <t>58</t>
+  </si>
+  <si>
+    <t>TOTAL HC</t>
   </si>
 </sst>
 </file>
@@ -869,7 +872,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -903,7 +906,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1218,10 +1221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B9F9AD4-448D-45CF-A558-F185D2C57E8E}">
-  <dimension ref="A1:M161"/>
+  <dimension ref="A1:M163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="D154" workbookViewId="0">
+      <selection activeCell="H163" sqref="H163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7833,6 +7836,23 @@
         <v>204</v>
       </c>
     </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A163" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F163" s="2">
+        <f t="shared" ref="F163:G163" si="0">SUM(F2:F161)</f>
+        <v>31154.694297059508</v>
+      </c>
+      <c r="G163" s="2">
+        <f t="shared" si="0"/>
+        <v>31202.219445813374</v>
+      </c>
+      <c r="H163" s="2">
+        <f>SUM(H2:H161)</f>
+        <v>28949.203359664763</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>